<commit_message>
Week 14 plus word para reader
</commit_message>
<xml_diff>
--- a/Plots/5 Atom System/Correlations/Propagation Speed/QMI Speed 5 atom.xlsx
+++ b/Plots/5 Atom System/Correlations/Propagation Speed/QMI Speed 5 atom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliverlind/Documents/Year 4 Project/L4ProgressGUI/Plots/5 Atom System/Correlations/Propagation Speed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CBD4A7-519E-C74B-9E43-A85C4FB59776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1607DD7E-CA28-2E4B-B84B-6C86E34169BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{96F0A57F-0DE6-2447-B153-979FA89E512E}"/>
   </bookViews>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFCB7058-D6C0-9949-B5CE-5D91A69FE288}">
   <dimension ref="A3:O216"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>